<commit_message>
Updates - add-delete holdings + email integration v1
</commit_message>
<xml_diff>
--- a/Final Project/api/data/imports/customers.xlsx
+++ b/Final Project/api/data/imports/customers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/227940f08aeb2ad5/Documents/GitHub/CIDM6330/Final Project/api/data/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{E0C11E5F-0867-4836-AD48-F1C3CA1D073D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E4DA5D-72D3-4D51-A67F-B7B4A78D0CF3}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{E0C11E5F-0867-4836-AD48-F1C3CA1D073D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF8F7AC5-3799-41AC-AAD1-1DEFAD27EAEA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{148EA2E9-DB15-4E93-91F0-336FADE7C8B6}"/>
+    <workbookView xWindow="32385" yWindow="3930" windowWidth="15360" windowHeight="11295" xr2:uid="{148EA2E9-DB15-4E93-91F0-336FADE7C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -90,13 +90,25 @@
   </si>
   <si>
     <t>customer_number</t>
+  </si>
+  <si>
+    <t>Jonathan Lowery</t>
+  </si>
+  <si>
+    <t>loweryjonf@gmail.com</t>
+  </si>
+  <si>
+    <t>salesperson_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salesperson_name </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +120,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,22 +150,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,110 +504,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA1129-F3A0-478D-935D-FC4EF9A991B5}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1014497</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>75001</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>540003</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>73301</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>540004</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>77001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{9ECDC6ED-570A-4084-BA01-C35C7C2ECFB3}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{12EA7732-9673-4509-9301-A74FF1C2C4B3}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{CCF0EEDC-6A0B-4DF8-9A4D-CA2B3F759FBE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>